<commit_message>
set defaults and get verify productfamily for the types
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf1310d49647bf51/PyCharmProjects/pricing-aws/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{978CC2CE-07B7-4B1B-B2F7-CF9339BF3E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D70BE4C3-261F-4205-AB3D-183CF7758E4B}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{978CC2CE-07B7-4B1B-B2F7-CF9339BF3E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A06BAB1-9920-4FA1-8D4D-B9E9D9CBB1D7}"/>
   <bookViews>
-    <workbookView xWindow="11865" yWindow="4125" windowWidth="21600" windowHeight="11385" xr2:uid="{8FD45EFC-8DC7-42EE-9B5A-6599DB738CBC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8FD45EFC-8DC7-42EE-9B5A-6599DB738CBC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ec2" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>instanceType</t>
   </si>
@@ -71,22 +71,10 @@
     <t>type</t>
   </si>
   <si>
-    <t>vm</t>
-  </si>
-  <si>
-    <t>tenancy</t>
-  </si>
-  <si>
     <t>Used</t>
   </si>
   <si>
-    <t>operatingsystem</t>
-  </si>
-  <si>
-    <t>Shared</t>
-  </si>
-  <si>
-    <t>RHEL</t>
+    <t>ec2</t>
   </si>
 </sst>
 </file>
@@ -442,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{934496E0-1C65-4DFF-9F5E-603C58A05CF7}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,10 +443,9 @@
     <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -477,16 +464,10 @@
       <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -495,7 +476,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -503,16 +484,10 @@
       <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -521,19 +496,13 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add support for multiple offers and pricing
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf1310d49647bf51/PyCharmProjects/pricing-aws/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{978CC2CE-07B7-4B1B-B2F7-CF9339BF3E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A06BAB1-9920-4FA1-8D4D-B9E9D9CBB1D7}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{978CC2CE-07B7-4B1B-B2F7-CF9339BF3E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC3AAC0C-1FDF-4B59-A66F-13D7D440208C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8FD45EFC-8DC7-42EE-9B5A-6599DB738CBC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8FD45EFC-8DC7-42EE-9B5A-6599DB738CBC}"/>
   </bookViews>
   <sheets>
     <sheet name="ec2" sheetId="1" r:id="rId1"/>
+    <sheet name="rds" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
   <si>
     <t>instanceType</t>
   </si>
@@ -75,6 +76,21 @@
   </si>
   <si>
     <t>ec2</t>
+  </si>
+  <si>
+    <t>us-gov-west-1</t>
+  </si>
+  <si>
+    <t>rds</t>
+  </si>
+  <si>
+    <t>db.r5.2xlarge</t>
+  </si>
+  <si>
+    <t>ebs</t>
+  </si>
+  <si>
+    <t>us-west-2</t>
   </si>
 </sst>
 </file>
@@ -430,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{934496E0-1C65-4DFF-9F5E-603C58A05CF7}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,6 +521,97 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD9B7A2A-1CF3-4E6E-89AB-DC93C5381E3E}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>